<commit_message>
- implementing max_race_count - adding 'polansky duatlonek', fixing zdechov
</commit_message>
<xml_diff>
--- a/2022/04-zdechov/krpál dospělí - VÝSLEDKY 2022.xlsx
+++ b/2022/04-zdechov/krpál dospělí - VÝSLEDKY 2022.xlsx
@@ -5,20 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CELKOVÉ VÝSLEDKY" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Muži 1" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Muži 2" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Muži 3" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Ženy 1" sheetId="5" state="hidden" r:id="rId6"/>
+    <sheet name="Ženy 1" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Ženy 2" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="JUNIOŘI" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Juniorky" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'CELKOVÉ VÝSLEDKY'!$A$2:$H$44</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Ženy 1'!$A$2:$I$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="123">
   <si>
     <t xml:space="preserve"> ZDĚCHOVSKÝ KRPÁL     2.7.2022</t>
   </si>
@@ -393,375 +393,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mikač</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BYDLIŠTĚ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kocourková</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ž2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zděchov 58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holzner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyrilometodějská 641, Valašské Klobouky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZVONEK SPORT VALAŠSKÉ KLOBOUKY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tomáš</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petříček</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nová Dědina, Kvasice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bike Triatlon Morkovice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miroslav</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janota</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hradská 254, Lukov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALACHBAJK TEAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zvonek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Záhumení 23, Val. Klobouky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ondřej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minařík</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Držková 149, Kašava</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V.I.K. Sport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fukala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horská 1921, Vsetín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALACH MTB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krejčí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rehak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pod Hájom 1083/38, Dubnica nad Váhom, SK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DUBNICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalousek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valašské Klobouky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZVONEK SPORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pavel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trňáček</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luční 4590, Zlín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flanderka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kunovice - Loučka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lukáš </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zapalač</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nový Hrozenkov 793</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otruba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veselská 5, Strážnice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OCELOVÍ LETCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">René </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slánský</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poteč</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYKLO MARTINEK - VALAŠSKÉ KLOBOUKY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chrástecký</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hovězí 710</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hečko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Na Honech 4910, Zlín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zdeněk </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skyba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otrokovice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TUFO CZ OTROKOVICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heryán</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bohuslavice u Zlína 257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSK VSETÍN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juřica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hovězí 682</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Držková, Kašava</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nehoda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jamnicz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dětmarovice 1353</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Husek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vídeňská 156, Medlovice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDLINE BIKE TEAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kvasnica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALMEZBIKE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baránek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Šerý</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bratří Hlaviců 69, Vsetín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALACHMTB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chocholáč</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palackého 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mikáč</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dohňany, SK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK EPIC DOHŇANY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AITES s.r.o.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petruj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Francova Lhota 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Šimara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huslenky 678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jaroslav</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smetana </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jasenná 167</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trlica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hovězí 47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lhotský</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louky 221, Zlín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SK LOUKY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Babiš</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mírová 1038, Bohumín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sekula </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zděchov 235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stanislav</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hajda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zděchov 219</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Novotný</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kroměříž</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stibora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bratří Hlaviců 109, Vsetín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kocourek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zděchov   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trochta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lidečko 467</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horní Lideč 209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plášek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rokytnice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALLTRAINING - LAWI - TEAM</t>
   </si>
   <si>
     <t xml:space="preserve">Staňka</t>
@@ -905,7 +536,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1038,18 +669,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1150,9 +769,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1189800</xdr:colOff>
+      <xdr:colOff>1189080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>732600</xdr:rowOff>
+      <xdr:rowOff>731880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1165,8 +784,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7272720" y="62280"/>
-          <a:ext cx="589680" cy="670320"/>
+          <a:off x="7272000" y="62280"/>
+          <a:ext cx="588960" cy="669600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1186,10 +805,10 @@
       <xdr:rowOff>62280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>614880</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>183960</xdr:rowOff>
+      <xdr:rowOff>183240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1202,8 +821,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9056880" y="10325160"/>
-          <a:ext cx="14040" cy="121680"/>
+          <a:off x="9056520" y="10325160"/>
+          <a:ext cx="14760" cy="120960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1229,9 +848,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1189800</xdr:colOff>
+      <xdr:colOff>1189080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>732600</xdr:rowOff>
+      <xdr:rowOff>731880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1244,8 +863,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8209800" y="62280"/>
-          <a:ext cx="589680" cy="670320"/>
+          <a:off x="8209440" y="62280"/>
+          <a:ext cx="588960" cy="669600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1271,9 +890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1189800</xdr:colOff>
+      <xdr:colOff>1189080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>732600</xdr:rowOff>
+      <xdr:rowOff>731880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1287,7 +906,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8613720" y="62280"/>
-          <a:ext cx="589680" cy="670320"/>
+          <a:ext cx="588960" cy="669600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,20 +925,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>600120</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>62280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1189800</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1189080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>732600</xdr:rowOff>
+      <xdr:rowOff>183240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Obrázek 2" descr=""/>
+        <xdr:cNvPr id="4" name="Obrázek 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1328,8 +947,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6547680" y="62280"/>
-          <a:ext cx="589680" cy="670320"/>
+          <a:off x="7858800" y="62280"/>
+          <a:ext cx="588960" cy="120960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1355,9 +974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1189800</xdr:colOff>
+      <xdr:colOff>1189080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>183960</xdr:rowOff>
+      <xdr:rowOff>183240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1370,8 +989,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7858080" y="62280"/>
-          <a:ext cx="589680" cy="121680"/>
+          <a:off x="7858800" y="62280"/>
+          <a:ext cx="588960" cy="120960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1397,12 +1016,12 @@
       <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.57"/>
@@ -2679,7 +2298,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.71"/>
@@ -3515,7 +3134,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.71"/>
@@ -3524,7 +3143,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.57"/>
   </cols>
   <sheetData>
@@ -4305,7 +3924,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="9.13"/>
@@ -5107,16 +4726,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.71"/>
@@ -5124,12 +4743,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="47.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5140,16 +4759,15 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -5159,1288 +4777,498 @@
         <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="27.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="33" t="n">
-        <v>0.0933101851851852</v>
-      </c>
-      <c r="C3" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" s="15" t="n">
-        <v>1976</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="33" t="n">
-        <v>0.0541319444444444</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>35</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G4" s="15" t="n">
-        <v>1992</v>
-      </c>
-      <c r="H4" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="33" t="n">
-        <v>0.0543171296296296</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="15" t="n">
-        <v>1990</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="33" t="n">
-        <v>0.0552893518518519</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>46</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G6" s="15" t="n">
-        <v>1977</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" s="33" t="n">
-        <v>0.0570949074074074</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <v>14</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G7" s="15" t="n">
-        <v>1984</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="33" t="n">
-        <v>0.057962962962963</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="15" t="n">
-        <v>1992</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="21.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="33" t="n">
-        <v>0.0600810185185185</v>
-      </c>
-      <c r="C9" s="6" t="n">
-        <v>39</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G9" s="15" t="n">
-        <v>1993</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="33" t="n">
-        <v>0.0598726851851852</v>
-      </c>
-      <c r="C10" s="6" t="n">
-        <v>43</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G10" s="15" t="n">
-        <v>1975</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="31.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" s="33" t="n">
-        <v>0.0627083333333333</v>
-      </c>
-      <c r="C11" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G11" s="15" t="n">
-        <v>1976</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="n">
-        <v>7</v>
-      </c>
-      <c r="B12" s="33" t="n">
-        <v>0.0606365740740741</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="15" t="n">
-        <v>1981</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="n">
-        <v>8</v>
-      </c>
-      <c r="B13" s="33" t="n">
-        <v>0.0628240740740741</v>
-      </c>
-      <c r="C13" s="6" t="n">
-        <v>41</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="15" t="n">
-        <v>1977</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="n">
-        <v>9</v>
-      </c>
-      <c r="B14" s="33" t="n">
-        <v>0.0633217592592593</v>
-      </c>
-      <c r="C14" s="6" t="n">
-        <v>37</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G14" s="15" t="n">
-        <v>1989</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="I14" s="15"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="30"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="30"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+    </row>
+    <row r="5" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="30"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="30"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="30"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="30"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="30"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="30"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="30"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="30"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="30"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="30"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="n">
-        <v>10</v>
-      </c>
-      <c r="B16" s="33" t="n">
-        <v>0.0633449074074074</v>
-      </c>
-      <c r="C16" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G16" s="15" t="n">
-        <v>1984</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G17" s="15" t="n">
-        <v>1944</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" s="33" t="n">
-        <v>0.0627662037037037</v>
-      </c>
-      <c r="C18" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G18" s="15" t="n">
-        <v>1972</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="n">
-        <v>11</v>
-      </c>
-      <c r="B19" s="33" t="n">
-        <v>0.0635648148148148</v>
-      </c>
-      <c r="C19" s="6" t="n">
-        <v>36</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G19" s="15" t="n">
-        <v>1996</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="n">
-        <v>12</v>
-      </c>
-      <c r="B20" s="33" t="n">
-        <v>0.0664351851851852</v>
-      </c>
-      <c r="C20" s="6" t="n">
-        <v>21</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" s="15" t="n">
-        <v>1987</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="n">
-        <v>13</v>
-      </c>
-      <c r="B21" s="33" t="n">
-        <v>0.0671064814814815</v>
-      </c>
-      <c r="C21" s="6" t="n">
-        <v>19</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" s="15" t="n">
-        <v>1999</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>182</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="30"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="30"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="30"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="30"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+    </row>
+    <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="30"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="30"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B23" s="33" t="n">
-        <v>0.0682407407407407</v>
-      </c>
-      <c r="C23" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G23" s="15" t="n">
-        <v>1987</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="n">
-        <v>15</v>
-      </c>
-      <c r="B24" s="33" t="n">
-        <v>0.0719212962962963</v>
-      </c>
-      <c r="C24" s="6" t="n">
-        <v>28</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="15" t="n">
-        <v>1989</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="I24" s="15"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="n">
-        <v>16</v>
-      </c>
-      <c r="B25" s="33" t="n">
-        <v>0.0726157407407407</v>
-      </c>
-      <c r="C25" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G25" s="15" t="n">
-        <v>1989</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="I25" s="15"/>
-    </row>
-    <row r="26" customFormat="false" ht="21.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="n">
-        <v>17</v>
-      </c>
-      <c r="B26" s="33" t="n">
-        <v>0.0738194444444444</v>
-      </c>
-      <c r="C26" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G26" s="15" t="n">
-        <v>1993</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="n">
-        <v>18</v>
-      </c>
-      <c r="B27" s="33" t="n">
-        <v>0.0742824074074074</v>
-      </c>
-      <c r="C27" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G27" s="15" t="n">
-        <v>1982</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="I27" s="15"/>
-    </row>
-    <row r="28" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="n">
-        <v>19</v>
-      </c>
-      <c r="B28" s="33" t="n">
-        <v>0.0751388888888889</v>
-      </c>
-      <c r="C28" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G28" s="15" t="n">
-        <v>1998</v>
-      </c>
-      <c r="H28" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="n">
-        <v>4</v>
-      </c>
-      <c r="B29" s="33" t="n">
-        <v>0.0681134259259259</v>
-      </c>
-      <c r="C29" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G29" s="15" t="n">
-        <v>1961</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="B30" s="33" t="n">
-        <v>0.0753587962962963</v>
-      </c>
-      <c r="C30" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G30" s="15" t="n">
-        <v>1983</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="I30" s="15"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="n">
-        <v>21</v>
-      </c>
-      <c r="B31" s="33" t="n">
-        <v>0.0764814814814815</v>
-      </c>
-      <c r="C31" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G31" s="15" t="n">
-        <v>1990</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="n">
-        <v>22</v>
-      </c>
-      <c r="B32" s="33" t="n">
-        <v>0.0793518518518519</v>
-      </c>
-      <c r="C32" s="6" t="n">
-        <v>42</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G32" s="15" t="n">
-        <v>1985</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="I32" s="15"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="n">
-        <v>5</v>
-      </c>
-      <c r="B33" s="33" t="n">
-        <v>0.0705092592592593</v>
-      </c>
-      <c r="C33" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33" s="15" t="n">
-        <v>1971</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="B34" s="33" t="n">
-        <v>0.071712962962963</v>
-      </c>
-      <c r="C34" s="6" t="n">
-        <v>32</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G34" s="15" t="n">
-        <v>1968</v>
-      </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15" t="s">
-        <v>211</v>
-      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="30"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="30"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="30"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="30"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="30"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="30"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="30"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="30"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="30"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="30"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="30"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="30"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="30"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="n">
-        <v>7</v>
-      </c>
-      <c r="B36" s="33" t="n">
-        <v>0.085162037037037</v>
-      </c>
-      <c r="C36" s="6" t="n">
-        <v>44</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G36" s="15" t="n">
-        <v>1968</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="I36" s="15"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15" t="n">
-        <v>23</v>
-      </c>
-      <c r="B37" s="33" t="n">
-        <v>0.0809375</v>
-      </c>
-      <c r="C37" s="6" t="n">
-        <v>17</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G37" s="15" t="n">
-        <v>1991</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="I37" s="15"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15" t="n">
-        <v>24</v>
-      </c>
-      <c r="B38" s="33" t="n">
-        <v>0.0810648148148148</v>
-      </c>
-      <c r="C38" s="6" t="n">
-        <v>47</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G38" s="15" t="n">
-        <v>1979</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="I38" s="15"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="15" t="n">
-        <v>25</v>
-      </c>
-      <c r="B39" s="33" t="n">
-        <v>0.0840393518518519</v>
-      </c>
-      <c r="C39" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G39" s="15" t="n">
-        <v>1987</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="I39" s="15"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="n">
-        <v>8</v>
-      </c>
-      <c r="B40" s="33" t="n">
-        <v>0.0864814814814815</v>
-      </c>
-      <c r="C40" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G40" s="15" t="n">
-        <v>1960</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="I40" s="15" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="15" t="n">
-        <v>26</v>
-      </c>
-      <c r="B41" s="33" t="n">
-        <v>0.0907523148148148</v>
-      </c>
-      <c r="C41" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G41" s="15" t="n">
-        <v>1982</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="I41" s="15"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="15" t="n">
-        <v>9</v>
-      </c>
-      <c r="B42" s="33" t="n">
-        <v>0.0872106481481482</v>
-      </c>
-      <c r="C42" s="6" t="n">
-        <v>40</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G42" s="15" t="n">
-        <v>1958</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="n">
-        <v>27</v>
-      </c>
-      <c r="B43" s="33" t="n">
-        <v>0.0953240740740741</v>
-      </c>
-      <c r="C43" s="6" t="n">
-        <v>45</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G43" s="15" t="n">
-        <v>1984</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="15" t="n">
-        <v>28</v>
-      </c>
-      <c r="B44" s="33" t="n">
-        <v>0.0964583333333333</v>
-      </c>
-      <c r="C44" s="6" t="n">
-        <v>23</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G44" s="15" t="n">
-        <v>1980</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="I44" s="35"/>
-    </row>
-    <row r="45" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="15" t="n">
-        <v>10</v>
-      </c>
-      <c r="B45" s="33" t="n">
-        <v>0.0896990740740741</v>
-      </c>
-      <c r="C45" s="6" t="n">
-        <v>38</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G45" s="15" t="n">
-        <v>1976</v>
-      </c>
-      <c r="H45" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="15" t="n">
-        <v>11</v>
-      </c>
-      <c r="B46" s="33" t="n">
-        <v>0.0977199074074074</v>
-      </c>
-      <c r="C46" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G46" s="15" t="n">
-        <v>1975</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="I46" s="15"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="15" t="n">
-        <v>29</v>
-      </c>
-      <c r="B47" s="33" t="n">
-        <v>0.0992476851851852</v>
-      </c>
-      <c r="C47" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="15" t="n">
-        <v>1987</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="I47" s="15"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="B48" s="33" t="n">
-        <v>0.104479166666667</v>
-      </c>
-      <c r="C48" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G48" s="15" t="n">
-        <v>1992</v>
-      </c>
-      <c r="H48" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="I48" s="15"/>
-    </row>
-    <row r="49" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G49" s="15" t="n">
-        <v>1994</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="I49" s="35" t="s">
-        <v>243</v>
-      </c>
-    </row>
+      <c r="B35" s="30"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="30"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="30"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="30"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="30"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="31"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="30"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="30"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="30"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="30"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="30"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="31"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A2:I49">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Ž1"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A3:I49">
-      <sortCondition ref="A3:A49" customList=""/>
-    </sortState>
-  </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -6464,7 +5292,7 @@
       <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.71"/>
@@ -6584,7 +5412,7 @@
         <v>114</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>244</v>
+        <v>121</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>110</v>
@@ -7135,11 +5963,11 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.3"/>
@@ -7318,7 +6146,7 @@
         <v>64</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>245</v>
+        <v>122</v>
       </c>
       <c r="F7" s="6" t="n">
         <v>2005</v>
@@ -7365,4 +6193,54 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>